<commit_message>
Fixed bug with non-greedy regular expression matching.
</commit_message>
<xml_diff>
--- a/Python/IssueTitleRefactoringDocCalculator/issue_title_refactoring_doc_text_patterns.csv.xlsx
+++ b/Python/IssueTitleRefactoringDocCalculator/issue_title_refactoring_doc_text_patterns.csv.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SmartSHARK\GitSmartSHARKfilePathconflict\SmartSHARKRepo\Python\IssueTitleRefactoringDocCalculator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{7629B4D4-4E0C-4415-B597-9C5F7643384A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFF8A532-27FF-4EC6-A4BC-A552EB676187}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Textual_patterns_issue_titles" sheetId="2" r:id="rId1"/>
@@ -131,7 +131,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1862,109 +1862,109 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="35"/>
                 <c:pt idx="0">
-                  <c:v>0.122349102773246</c:v>
+                  <c:v>3.7792895E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0.11337868500000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.6916802610114101</c:v>
-                </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.1566068515497497E-2</c:v>
+                  <c:v>3.0990173849999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>30.7096247960848</c:v>
+                  <c:v>0.15117158</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.2202283849918398</c:v>
+                  <c:v>29.402872259999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.4420880913539893</c:v>
+                  <c:v>5.5555555559999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.8140293637846598</c:v>
+                  <c:v>8.6545729399999995</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.6101141924959199</c:v>
+                  <c:v>2.8722600150000002</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7.4632952691680199</c:v>
+                  <c:v>2.9856387</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10.0326264274062</c:v>
+                  <c:v>7.2184429330000004</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.48939641109298498</c:v>
+                  <c:v>9.4860166289999999</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.0603588907014601</c:v>
+                  <c:v>0.453514739</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.4061990212071702</c:v>
+                  <c:v>1.1715797429999999</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.7928221859706301</c:v>
+                  <c:v>2.456538171</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4.07830342577487E-2</c:v>
+                  <c:v>3.741496599</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.24469820554649199</c:v>
+                  <c:v>3.7792895E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.5905383360522001</c:v>
+                  <c:v>0.22675737000000001</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.48939641109298498</c:v>
+                  <c:v>1.9274376419999999</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>10.0326264274062</c:v>
+                  <c:v>0.453514739</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.9575856443719399</c:v>
+                  <c:v>9.9773242629999999</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.122349102773246</c:v>
+                  <c:v>1.9652305370000001</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>3.3849918433931401</c:v>
+                  <c:v>0.11337868500000001</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>4.07830342577487E-2</c:v>
+                  <c:v>3.439153439</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1.4681892332789499</c:v>
+                  <c:v>1.5495086920000001</c:v>
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.16313213703099499</c:v>
+                  <c:v>0.15117158</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1.6313213703099501</c:v>
+                  <c:v>1.700680272</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.24469820554649199</c:v>
+                  <c:v>0.22675737000000001</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0</c:v>
+                  <c:v>3.7792895E-2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0</c:v>
+                  <c:v>0.11337868500000001</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0</c:v>
+                  <c:v>3.7792895E-2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.122349102773246</c:v>
+                  <c:v>0.11337868500000001</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.448613376835236</c:v>
+                  <c:v>0.453514739</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>8.1566068515497497E-2</c:v>
+                  <c:v>7.558579E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2727,10 +2727,10 @@
 </file>
 
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" workbookViewId="0"/>
+    <sheetView zoomScale="130" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2741,7 +2741,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8668987" cy="6264234"/>
+    <xdr:ext cx="8669215" cy="6260123"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -3066,11 +3066,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AI2"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="69" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AK28" sqref="AK28"/>
+    <sheetView tabSelected="1" zoomScale="43" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AI1" sqref="A1:AI2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3184,109 +3184,109 @@
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>0.122349102773246</v>
+        <v>3.7792895E-2</v>
       </c>
       <c r="B2">
+        <v>0.11337868500000001</v>
+      </c>
+      <c r="C2">
         <v>0</v>
       </c>
-      <c r="C2">
-        <v>2.6916802610114101</v>
-      </c>
       <c r="D2">
-        <v>8.1566068515497497E-2</v>
+        <v>3.0990173849999998</v>
       </c>
       <c r="E2">
-        <v>30.7096247960848</v>
+        <v>0.15117158</v>
       </c>
       <c r="F2">
-        <v>5.2202283849918398</v>
+        <v>29.402872259999999</v>
       </c>
       <c r="G2">
-        <v>8.4420880913539893</v>
+        <v>5.5555555559999998</v>
       </c>
       <c r="H2">
-        <v>2.8140293637846598</v>
+        <v>8.6545729399999995</v>
       </c>
       <c r="I2">
-        <v>2.6101141924959199</v>
+        <v>2.8722600150000002</v>
       </c>
       <c r="J2">
-        <v>7.4632952691680199</v>
+        <v>2.9856387</v>
       </c>
       <c r="K2">
-        <v>10.0326264274062</v>
+        <v>7.2184429330000004</v>
       </c>
       <c r="L2">
-        <v>0.48939641109298498</v>
+        <v>9.4860166289999999</v>
       </c>
       <c r="M2">
-        <v>1.0603588907014601</v>
+        <v>0.453514739</v>
       </c>
       <c r="N2">
-        <v>2.4061990212071702</v>
+        <v>1.1715797429999999</v>
       </c>
       <c r="O2">
-        <v>3.7928221859706301</v>
+        <v>2.456538171</v>
       </c>
       <c r="P2">
-        <v>4.07830342577487E-2</v>
+        <v>3.741496599</v>
       </c>
       <c r="Q2">
-        <v>0.24469820554649199</v>
+        <v>3.7792895E-2</v>
       </c>
       <c r="R2">
-        <v>1.5905383360522001</v>
+        <v>0.22675737000000001</v>
       </c>
       <c r="S2">
-        <v>0.48939641109298498</v>
+        <v>1.9274376419999999</v>
       </c>
       <c r="T2">
-        <v>10.0326264274062</v>
+        <v>0.453514739</v>
       </c>
       <c r="U2">
-        <v>1.9575856443719399</v>
+        <v>9.9773242629999999</v>
       </c>
       <c r="V2">
-        <v>0.122349102773246</v>
+        <v>1.9652305370000001</v>
       </c>
       <c r="W2">
-        <v>3.3849918433931401</v>
+        <v>0.11337868500000001</v>
       </c>
       <c r="X2">
-        <v>4.07830342577487E-2</v>
+        <v>3.439153439</v>
       </c>
       <c r="Y2">
-        <v>1.4681892332789499</v>
+        <v>1.5495086920000001</v>
       </c>
       <c r="Z2">
         <v>0</v>
       </c>
       <c r="AA2">
-        <v>0.16313213703099499</v>
+        <v>0.15117158</v>
       </c>
       <c r="AB2">
-        <v>1.6313213703099501</v>
+        <v>1.700680272</v>
       </c>
       <c r="AC2">
-        <v>0.24469820554649199</v>
+        <v>0.22675737000000001</v>
       </c>
       <c r="AD2">
-        <v>0</v>
+        <v>3.7792895E-2</v>
       </c>
       <c r="AE2">
-        <v>0</v>
+        <v>0.11337868500000001</v>
       </c>
       <c r="AF2">
-        <v>0</v>
+        <v>3.7792895E-2</v>
       </c>
       <c r="AG2">
-        <v>0.122349102773246</v>
+        <v>0.11337868500000001</v>
       </c>
       <c r="AH2">
-        <v>0.448613376835236</v>
+        <v>0.453514739</v>
       </c>
       <c r="AI2">
-        <v>8.1566068515497497E-2</v>
+        <v>7.558579E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Regenerated the output CSV file issue title refactoring documentation with a greedy reg exp search.
</commit_message>
<xml_diff>
--- a/Python/IssueTitleRefactoringDocCalculator/issue_title_refactoring_doc_text_patterns.csv.xlsx
+++ b/Python/IssueTitleRefactoringDocCalculator/issue_title_refactoring_doc_text_patterns.csv.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SmartSHARK\GitSmartSHARKfilePathconflict\SmartSHARKRepo\Python\IssueTitleRefactoringDocCalculator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFF8A532-27FF-4EC6-A4BC-A552EB676187}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D85484AE-5056-45DA-907E-4B56A52E7DD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1862,109 +1862,109 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="35"/>
                 <c:pt idx="0">
-                  <c:v>3.7792895E-2</c:v>
+                  <c:v>3.7792894935751997E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.11337868500000001</c:v>
+                  <c:v>0.11337868480725601</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.0990173849999998</c:v>
+                  <c:v>3.09901738473167</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.15117158</c:v>
+                  <c:v>0.15117157974300799</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>29.402872259999999</c:v>
+                  <c:v>29.402872260015101</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.5555555559999998</c:v>
+                  <c:v>5.55555555555555</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8.6545729399999995</c:v>
+                  <c:v>8.6545729402872205</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.8722600150000002</c:v>
+                  <c:v>2.87226001511715</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.9856387</c:v>
+                  <c:v>2.9856386999244098</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>7.2184429330000004</c:v>
+                  <c:v>7.2184429327286397</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>9.4860166289999999</c:v>
+                  <c:v>9.4860166288737702</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.453514739</c:v>
+                  <c:v>0.45351473922902402</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.1715797429999999</c:v>
+                  <c:v>1.1715797430083099</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.456538171</c:v>
+                  <c:v>2.45653817082388</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3.741496599</c:v>
+                  <c:v>3.7414965986394502</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3.7792895E-2</c:v>
+                  <c:v>3.7792894935751997E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.22675737000000001</c:v>
+                  <c:v>0.22675736961451201</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.9274376419999999</c:v>
+                  <c:v>1.9274376417233501</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.453514739</c:v>
+                  <c:v>0.45351473922902402</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>9.9773242629999999</c:v>
+                  <c:v>9.9773242630385397</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1.9652305370000001</c:v>
+                  <c:v>1.9652305366591001</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.11337868500000001</c:v>
+                  <c:v>0.11337868480725601</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>3.439153439</c:v>
+                  <c:v>3.4391534391534302</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1.5495086920000001</c:v>
+                  <c:v>1.5495086923658301</c:v>
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.15117158</c:v>
+                  <c:v>0.15117157974300799</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1.700680272</c:v>
+                  <c:v>1.7006802721088401</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.22675737000000001</c:v>
+                  <c:v>0.22675736961451201</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>3.7792895E-2</c:v>
+                  <c:v>3.7792894935751997E-2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.11337868500000001</c:v>
+                  <c:v>0.11337868480725601</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>3.7792895E-2</c:v>
+                  <c:v>3.7792894935751997E-2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.11337868500000001</c:v>
+                  <c:v>0.11337868480725601</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.453514739</c:v>
+                  <c:v>0.45351473922902402</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>7.558579E-2</c:v>
+                  <c:v>7.5585789871504105E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3070,7 +3070,7 @@
   <dimension ref="A1:AI2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="43" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AI1" sqref="A1:AI2"/>
+      <selection sqref="A1:AI2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3184,109 +3184,109 @@
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>3.7792895E-2</v>
+        <v>3.7792894935751997E-2</v>
       </c>
       <c r="B2">
-        <v>0.11337868500000001</v>
+        <v>0.11337868480725601</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2">
-        <v>3.0990173849999998</v>
+        <v>3.09901738473167</v>
       </c>
       <c r="E2">
-        <v>0.15117158</v>
+        <v>0.15117157974300799</v>
       </c>
       <c r="F2">
-        <v>29.402872259999999</v>
+        <v>29.402872260015101</v>
       </c>
       <c r="G2">
-        <v>5.5555555559999998</v>
+        <v>5.55555555555555</v>
       </c>
       <c r="H2">
-        <v>8.6545729399999995</v>
+        <v>8.6545729402872205</v>
       </c>
       <c r="I2">
-        <v>2.8722600150000002</v>
+        <v>2.87226001511715</v>
       </c>
       <c r="J2">
-        <v>2.9856387</v>
+        <v>2.9856386999244098</v>
       </c>
       <c r="K2">
-        <v>7.2184429330000004</v>
+        <v>7.2184429327286397</v>
       </c>
       <c r="L2">
-        <v>9.4860166289999999</v>
+        <v>9.4860166288737702</v>
       </c>
       <c r="M2">
-        <v>0.453514739</v>
+        <v>0.45351473922902402</v>
       </c>
       <c r="N2">
-        <v>1.1715797429999999</v>
+        <v>1.1715797430083099</v>
       </c>
       <c r="O2">
-        <v>2.456538171</v>
+        <v>2.45653817082388</v>
       </c>
       <c r="P2">
-        <v>3.741496599</v>
+        <v>3.7414965986394502</v>
       </c>
       <c r="Q2">
-        <v>3.7792895E-2</v>
+        <v>3.7792894935751997E-2</v>
       </c>
       <c r="R2">
-        <v>0.22675737000000001</v>
+        <v>0.22675736961451201</v>
       </c>
       <c r="S2">
-        <v>1.9274376419999999</v>
+        <v>1.9274376417233501</v>
       </c>
       <c r="T2">
-        <v>0.453514739</v>
+        <v>0.45351473922902402</v>
       </c>
       <c r="U2">
-        <v>9.9773242629999999</v>
+        <v>9.9773242630385397</v>
       </c>
       <c r="V2">
-        <v>1.9652305370000001</v>
+        <v>1.9652305366591001</v>
       </c>
       <c r="W2">
-        <v>0.11337868500000001</v>
+        <v>0.11337868480725601</v>
       </c>
       <c r="X2">
-        <v>3.439153439</v>
+        <v>3.4391534391534302</v>
       </c>
       <c r="Y2">
-        <v>1.5495086920000001</v>
+        <v>1.5495086923658301</v>
       </c>
       <c r="Z2">
         <v>0</v>
       </c>
       <c r="AA2">
-        <v>0.15117158</v>
+        <v>0.15117157974300799</v>
       </c>
       <c r="AB2">
-        <v>1.700680272</v>
+        <v>1.7006802721088401</v>
       </c>
       <c r="AC2">
-        <v>0.22675737000000001</v>
+        <v>0.22675736961451201</v>
       </c>
       <c r="AD2">
-        <v>3.7792895E-2</v>
+        <v>3.7792894935751997E-2</v>
       </c>
       <c r="AE2">
-        <v>0.11337868500000001</v>
+        <v>0.11337868480725601</v>
       </c>
       <c r="AF2">
-        <v>3.7792895E-2</v>
+        <v>3.7792894935751997E-2</v>
       </c>
       <c r="AG2">
-        <v>0.11337868500000001</v>
+        <v>0.11337868480725601</v>
       </c>
       <c r="AH2">
-        <v>0.453514739</v>
+        <v>0.45351473922902402</v>
       </c>
       <c r="AI2">
-        <v>7.558579E-2</v>
+        <v>7.5585789871504105E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rewrote main module in IssueTitleRefactoringDocCalculator to not count the same issue more than once.
</commit_message>
<xml_diff>
--- a/Python/IssueTitleRefactoringDocCalculator/issue_title_refactoring_doc_text_patterns.csv.xlsx
+++ b/Python/IssueTitleRefactoringDocCalculator/issue_title_refactoring_doc_text_patterns.csv.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SmartSHARK\GitSmartSHARKfilePathconflict\SmartSHARKRepo\Python\IssueTitleRefactoringDocCalculator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D85484AE-5056-45DA-907E-4B56A52E7DD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5063F69F-2E49-4143-8910-636C4AA2704C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Textual_patterns_issue_titles" sheetId="2" r:id="rId1"/>
@@ -1862,109 +1862,109 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="35"/>
                 <c:pt idx="0">
-                  <c:v>3.7792894935751997E-2</c:v>
+                  <c:v>3.7792895E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.11337868480725601</c:v>
+                  <c:v>0.11337868500000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.09901738473167</c:v>
+                  <c:v>3.0990173849999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.15117157974300799</c:v>
+                  <c:v>0.15117158</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>29.402872260015101</c:v>
+                  <c:v>29.402872259999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.55555555555555</c:v>
+                  <c:v>5.5555555559999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8.6545729402872205</c:v>
+                  <c:v>8.6545729399999995</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.87226001511715</c:v>
+                  <c:v>2.8722600150000002</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.9856386999244098</c:v>
+                  <c:v>2.9856387</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>7.2184429327286397</c:v>
+                  <c:v>7.2184429330000004</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>9.4860166288737702</c:v>
+                  <c:v>9.4860166289999999</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.45351473922902402</c:v>
+                  <c:v>0.453514739</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.1715797430083099</c:v>
+                  <c:v>1.1715797429999999</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.45653817082388</c:v>
+                  <c:v>2.456538171</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3.7414965986394502</c:v>
+                  <c:v>3.741496599</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3.7792894935751997E-2</c:v>
+                  <c:v>3.7792895E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.22675736961451201</c:v>
+                  <c:v>0.22675737000000001</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.9274376417233501</c:v>
+                  <c:v>1.9274376419999999</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.45351473922902402</c:v>
+                  <c:v>0.453514739</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>9.9773242630385397</c:v>
+                  <c:v>9.9773242629999999</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1.9652305366591001</c:v>
+                  <c:v>1.9652305370000001</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.11337868480725601</c:v>
+                  <c:v>0.11337868500000001</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>3.4391534391534302</c:v>
+                  <c:v>3.439153439</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1.5495086923658301</c:v>
+                  <c:v>1.5495086920000001</c:v>
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.15117157974300799</c:v>
+                  <c:v>0.15117158</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1.7006802721088401</c:v>
+                  <c:v>1.700680272</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.22675736961451201</c:v>
+                  <c:v>0.22675737000000001</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>3.7792894935751997E-2</c:v>
+                  <c:v>3.7792895E-2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.11337868480725601</c:v>
+                  <c:v>0.11337868500000001</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>3.7792894935751997E-2</c:v>
+                  <c:v>3.7792895E-2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.11337868480725601</c:v>
+                  <c:v>0.11337868500000001</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.45351473922902402</c:v>
+                  <c:v>0.453514739</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>7.5585789871504105E-2</c:v>
+                  <c:v>7.558579E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2730,7 +2730,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="130" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="130" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3069,7 +3069,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AI2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="43" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView zoomScale="43" zoomScaleNormal="55" workbookViewId="0">
       <selection sqref="A1:AI2"/>
     </sheetView>
   </sheetViews>
@@ -3184,109 +3184,109 @@
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>3.7792894935751997E-2</v>
+        <v>3.7792895E-2</v>
       </c>
       <c r="B2">
-        <v>0.11337868480725601</v>
+        <v>0.11337868500000001</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2">
-        <v>3.09901738473167</v>
+        <v>3.0990173849999998</v>
       </c>
       <c r="E2">
-        <v>0.15117157974300799</v>
+        <v>0.15117158</v>
       </c>
       <c r="F2">
-        <v>29.402872260015101</v>
+        <v>29.402872259999999</v>
       </c>
       <c r="G2">
-        <v>5.55555555555555</v>
+        <v>5.5555555559999998</v>
       </c>
       <c r="H2">
-        <v>8.6545729402872205</v>
+        <v>8.6545729399999995</v>
       </c>
       <c r="I2">
-        <v>2.87226001511715</v>
+        <v>2.8722600150000002</v>
       </c>
       <c r="J2">
-        <v>2.9856386999244098</v>
+        <v>2.9856387</v>
       </c>
       <c r="K2">
-        <v>7.2184429327286397</v>
+        <v>7.2184429330000004</v>
       </c>
       <c r="L2">
-        <v>9.4860166288737702</v>
+        <v>9.4860166289999999</v>
       </c>
       <c r="M2">
-        <v>0.45351473922902402</v>
+        <v>0.453514739</v>
       </c>
       <c r="N2">
-        <v>1.1715797430083099</v>
+        <v>1.1715797429999999</v>
       </c>
       <c r="O2">
-        <v>2.45653817082388</v>
+        <v>2.456538171</v>
       </c>
       <c r="P2">
-        <v>3.7414965986394502</v>
+        <v>3.741496599</v>
       </c>
       <c r="Q2">
-        <v>3.7792894935751997E-2</v>
+        <v>3.7792895E-2</v>
       </c>
       <c r="R2">
-        <v>0.22675736961451201</v>
+        <v>0.22675737000000001</v>
       </c>
       <c r="S2">
-        <v>1.9274376417233501</v>
+        <v>1.9274376419999999</v>
       </c>
       <c r="T2">
-        <v>0.45351473922902402</v>
+        <v>0.453514739</v>
       </c>
       <c r="U2">
-        <v>9.9773242630385397</v>
+        <v>9.9773242629999999</v>
       </c>
       <c r="V2">
-        <v>1.9652305366591001</v>
+        <v>1.9652305370000001</v>
       </c>
       <c r="W2">
-        <v>0.11337868480725601</v>
+        <v>0.11337868500000001</v>
       </c>
       <c r="X2">
-        <v>3.4391534391534302</v>
+        <v>3.439153439</v>
       </c>
       <c r="Y2">
-        <v>1.5495086923658301</v>
+        <v>1.5495086920000001</v>
       </c>
       <c r="Z2">
         <v>0</v>
       </c>
       <c r="AA2">
-        <v>0.15117157974300799</v>
+        <v>0.15117158</v>
       </c>
       <c r="AB2">
-        <v>1.7006802721088401</v>
+        <v>1.700680272</v>
       </c>
       <c r="AC2">
-        <v>0.22675736961451201</v>
+        <v>0.22675737000000001</v>
       </c>
       <c r="AD2">
-        <v>3.7792894935751997E-2</v>
+        <v>3.7792895E-2</v>
       </c>
       <c r="AE2">
-        <v>0.11337868480725601</v>
+        <v>0.11337868500000001</v>
       </c>
       <c r="AF2">
-        <v>3.7792894935751997E-2</v>
+        <v>3.7792895E-2</v>
       </c>
       <c r="AG2">
-        <v>0.11337868480725601</v>
+        <v>0.11337868500000001</v>
       </c>
       <c r="AH2">
-        <v>0.45351473922902402</v>
+        <v>0.453514739</v>
       </c>
       <c r="AI2">
-        <v>7.5585789871504105E-2</v>
+        <v>7.558579E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>